<commit_message>
Schema update - proper impementation of alignment tree in core
</commit_message>
<xml_diff>
--- a/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/AAV-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CCCEB9-6269-D448-8219-E305946ABFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F90BC1-DAA5-D942-9159-7FE7BF68B00F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="5740" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parvo-ncbi-refseqs-side-data" sheetId="1" r:id="rId1"/>
+    <sheet name="to add" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="73">
   <si>
     <t>virus_name</t>
   </si>
@@ -221,6 +222,24 @@
   </si>
   <si>
     <t>Dependo3</t>
+  </si>
+  <si>
+    <t>virus_subfamily</t>
+  </si>
+  <si>
+    <t>Parvovirinae</t>
+  </si>
+  <si>
+    <t>Densovirinae</t>
+  </si>
+  <si>
+    <t>Hamaparvovirinae</t>
+  </si>
+  <si>
+    <t>Ichthamaparvovirus</t>
+  </si>
+  <si>
+    <t>GpChPV</t>
   </si>
 </sst>
 </file>
@@ -363,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +565,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF660066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,9 +747,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,18 +1108,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:K17"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1090,571 +1132,619 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F14" t="s">
         <v>66</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G14" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H14" t="s">
         <v>66</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I14" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J14" t="s">
         <v>66</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K14" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
@@ -1671,10 +1761,49 @@
         <v>13</v>
       </c>
       <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+    <sortCondition ref="D2:D17"/>
+    <sortCondition ref="E2:E17"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A294D4-B9B4-0343-89CB-D84830908F70}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added genus Artiparvovirus to core build
</commit_message>
<xml_diff>
--- a/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838F13AB-853F-3242-807B-393B89C3FFFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA9EDE7-2A16-D344-BD63-34A5AE2A7220}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="119">
   <si>
     <t>virus_name</t>
   </si>
@@ -342,6 +342,42 @@
   </si>
   <si>
     <t>Pefuambidensovirus</t>
+  </si>
+  <si>
+    <t>Eidolon helvum parvovirus 1</t>
+  </si>
+  <si>
+    <t>NC_007018</t>
+  </si>
+  <si>
+    <t>Human parvovirus 4</t>
+  </si>
+  <si>
+    <t>Carnivore protoparvovirus</t>
+  </si>
+  <si>
+    <t>PARV4</t>
+  </si>
+  <si>
+    <t>Bovine parvovirus 2</t>
+  </si>
+  <si>
+    <t>Bovine parvovirus</t>
+  </si>
+  <si>
+    <t>Chicken parvovirus</t>
+  </si>
+  <si>
+    <t>Porcine parvovirus 7</t>
+  </si>
+  <si>
+    <t>Fenneropenaeus chinensis hepatopancreatic densovirus</t>
+  </si>
+  <si>
+    <t>Infectious hypodermal and hematopoietic necrosis virus</t>
+  </si>
+  <si>
+    <t>Aedes albopictus densovirus 2</t>
   </si>
 </sst>
 </file>
@@ -1210,15 +1246,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:L24"/>
+      <selection activeCell="C21" sqref="A1:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
@@ -1583,7 +1619,7 @@
         <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
@@ -1615,7 +1651,7 @@
         <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>68</v>
@@ -1653,7 +1689,7 @@
         <v>62</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>68</v>
@@ -1691,7 +1727,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>68</v>
@@ -1767,7 +1803,7 @@
         <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>68</v>
@@ -1843,7 +1879,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>66</v>
@@ -1881,7 +1917,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>66</v>
@@ -1919,7 +1955,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>66</v>
@@ -2071,7 +2107,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>66</v>
@@ -2109,33 +2145,71 @@
         <v>44</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24" s="4" t="s">
+      <c r="F25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor - extra directory level for EVE tabular data
</commit_message>
<xml_diff>
--- a/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8CFE86-8137-6F41-BFF8-4EF34BC56C7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C01691F-1DC9-9446-8EA8-A84CD4FAEE0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22820" yWindow="740" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1257,7 +1257,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Include HHV-6  Rep (U6) in core
</commit_message>
<xml_diff>
--- a/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C01691F-1DC9-9446-8EA8-A84CD4FAEE0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D62521-A139-764F-8A0E-ECD19B4355D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22820" yWindow="740" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="122">
   <si>
     <t>virus_name</t>
   </si>
@@ -375,6 +375,18 @@
   </si>
   <si>
     <t>Aedes albopictus densovirus 2</t>
+  </si>
+  <si>
+    <t>X59532</t>
+  </si>
+  <si>
+    <t>HHV6-Rep</t>
+  </si>
+  <si>
+    <t>Betherpesparvovirus</t>
+  </si>
+  <si>
+    <t>Proto1</t>
   </si>
 </sst>
 </file>
@@ -1254,14 +1266,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="52.83203125" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="33.1640625" customWidth="1"/>
@@ -2124,22 +2138,22 @@
         <v>27</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>13</v>
@@ -2218,6 +2232,44 @@
         <v>13</v>
       </c>
       <c r="L25" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor - bring Copi component into align tree
</commit_message>
<xml_diff>
--- a/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/parvo-ncbi-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D67879-6CD0-0247-8FC9-0884745694B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22617505-4491-1D41-ACFB-7559C1ACD526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="500" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>